<commit_message>
confidene interval save 1
</commit_message>
<xml_diff>
--- a/content/downloads/notebooks/negative_sampling.xlsx
+++ b/content/downloads/notebooks/negative_sampling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricKim\Documents\aegis4048.github.io-source\content\downloads\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01100567-58BF-437E-B2A9-7D392EBAF385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A142BA-A730-4BF4-8056-BDDDDF2ADF0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" firstSheet="1" activeTab="11" xr2:uid="{C6B97615-1AA9-4D30-82D3-AEB364AF5D74}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -918,24 +918,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1056,18 +1038,6 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1154,6 +1124,24 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4106,8 +4094,8 @@
       <xdr:rowOff>58495</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="454868" cy="235706"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -4209,7 +4197,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -4274,8 +4262,8 @@
       <xdr:rowOff>277901</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -4339,7 +4327,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -4405,8 +4393,8 @@
       <xdr:rowOff>277907</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4470,7 +4458,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4536,8 +4524,8 @@
       <xdr:rowOff>94129</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="546111" cy="184794"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -4651,7 +4639,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -4724,8 +4712,8 @@
       <xdr:rowOff>278643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4789,7 +4777,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4855,8 +4843,8 @@
       <xdr:rowOff>64194</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="466281" cy="235706"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -4958,7 +4946,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -5023,8 +5011,8 @@
       <xdr:rowOff>58495</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="519116" cy="231923"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -5126,7 +5114,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -5191,8 +5179,8 @@
       <xdr:rowOff>94129</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="567143" cy="184794"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -5306,7 +5294,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -5378,7 +5366,7 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>64194</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="466281" cy="235706"/>
+    <xdr:ext cx="519116" cy="231923"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -5395,7 +5383,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7954314" y="4072314"/>
-              <a:ext cx="466281" cy="235706"/>
+              <a:ext cx="519116" cy="231923"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5450,7 +5438,7 @@
                           <a:rPr lang="en-US" sz="1100" b="1" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>𝒊𝒏𝒑𝒖𝒕</m:t>
+                          <m:t>𝒐𝒖𝒕𝒑𝒖𝒕</m:t>
                         </m:r>
                       </m:sub>
                       <m:sup>
@@ -5497,7 +5485,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7954314" y="4072314"/>
-              <a:ext cx="466281" cy="235706"/>
+              <a:ext cx="519116" cy="231923"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5529,7 +5517,7 @@
                 <a:rPr lang="en-US" sz="1100" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑾_𝒊𝒏𝒑𝒖𝒕^((𝒏𝒆𝒘))</a:t>
+                <a:t>𝑾_𝒐𝒖𝒕𝒑𝒖𝒕^((𝒏𝒆𝒘))</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="1"/>
             </a:p>
@@ -5547,8 +5535,8 @@
       <xdr:rowOff>277200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -5612,7 +5600,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -5678,8 +5666,8 @@
       <xdr:rowOff>277206</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -5743,7 +5731,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -5809,8 +5797,8 @@
       <xdr:rowOff>277942</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -5874,7 +5862,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -12019,9 +12007,9 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>64194</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="466281" cy="235706"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="519116" cy="231923"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -12035,8 +12023,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7937571" y="611546"/>
-              <a:ext cx="466281" cy="235706"/>
+              <a:off x="7954314" y="4072314"/>
+              <a:ext cx="519116" cy="231923"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12091,7 +12079,7 @@
                           <a:rPr lang="en-US" sz="1100" b="1" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>𝒊𝒏𝒑𝒖𝒕</m:t>
+                          <m:t>𝒐𝒖𝒕𝒑𝒖𝒕</m:t>
                         </m:r>
                       </m:sub>
                       <m:sup>
@@ -12123,7 +12111,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -12137,8 +12125,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7937571" y="611546"/>
-              <a:ext cx="466281" cy="235706"/>
+              <a:off x="7954314" y="4072314"/>
+              <a:ext cx="519116" cy="231923"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12165,11 +12153,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑾_𝒊𝒏𝒑𝒖𝒕^((𝒏𝒆𝒘))</a:t>
+                <a:t>𝑾_𝒐𝒖𝒕𝒑𝒖𝒕^((𝒏𝒆𝒘))</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="1"/>
             </a:p>
@@ -16167,43 +16156,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
     </row>
     <row r="4" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
     </row>
     <row r="5" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
     </row>
     <row r="6" spans="2:10" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1"/>
@@ -16244,7 +16233,7 @@
       <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E8" s="76"/>
+      <c r="E8" s="145"/>
       <c r="F8" s="46">
         <v>-1.4E-2</v>
       </c>
@@ -16254,7 +16243,7 @@
       <c r="H8" s="46">
         <v>0.109</v>
       </c>
-      <c r="I8" s="76"/>
+      <c r="I8" s="145"/>
       <c r="J8" s="7">
         <f t="array" ref="J8:J10">TRANSPOSE(MMULT(TRANSPOSE(input), w_input))</f>
         <v>-1.7999999999999999E-2</v>
@@ -16270,7 +16259,7 @@
       <c r="D9" s="9">
         <v>0</v>
       </c>
-      <c r="E9" s="76"/>
+      <c r="E9" s="145"/>
       <c r="F9" s="46">
         <v>-0.66500000000000004</v>
       </c>
@@ -16280,7 +16269,7 @@
       <c r="H9" s="46">
         <v>0.309</v>
       </c>
-      <c r="I9" s="76"/>
+      <c r="I9" s="145"/>
       <c r="J9" s="7">
         <v>0.40400000000000003</v>
       </c>
@@ -16295,7 +16284,7 @@
       <c r="D10" s="11">
         <v>0</v>
       </c>
-      <c r="E10" s="76"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="46">
         <v>0.70199999999999996</v>
       </c>
@@ -16305,7 +16294,7 @@
       <c r="H10" s="46">
         <v>-0.98099999999999998</v>
       </c>
-      <c r="I10" s="76"/>
+      <c r="I10" s="145"/>
       <c r="J10" s="7">
         <v>-0.317</v>
       </c>
@@ -16320,7 +16309,7 @@
       <c r="D11" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="76"/>
+      <c r="E11" s="145"/>
       <c r="F11" s="46">
         <v>0.214</v>
       </c>
@@ -16330,7 +16319,7 @@
       <c r="H11" s="46">
         <v>-0.56100000000000005</v>
       </c>
-      <c r="I11" s="76"/>
+      <c r="I11" s="145"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -16343,17 +16332,17 @@
       <c r="D12" s="20">
         <v>1</v>
       </c>
-      <c r="E12" s="76"/>
-      <c r="F12" s="151">
+      <c r="E12" s="145"/>
+      <c r="F12" s="141">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="G12" s="151">
+      <c r="G12" s="141">
         <v>0.40400000000000003</v>
       </c>
-      <c r="H12" s="151">
+      <c r="H12" s="141">
         <v>-0.317</v>
       </c>
-      <c r="I12" s="76"/>
+      <c r="I12" s="145"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -16366,7 +16355,7 @@
       <c r="D13" s="14">
         <v>0</v>
       </c>
-      <c r="E13" s="76"/>
+      <c r="E13" s="145"/>
       <c r="F13" s="46">
         <v>0.20399999999999999</v>
       </c>
@@ -16376,7 +16365,7 @@
       <c r="H13" s="46">
         <v>-0.73299999999999998</v>
       </c>
-      <c r="I13" s="76"/>
+      <c r="I13" s="145"/>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -16389,7 +16378,7 @@
       <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="76"/>
+      <c r="E14" s="145"/>
       <c r="F14" s="46">
         <v>-0.65200000000000002</v>
       </c>
@@ -16399,7 +16388,7 @@
       <c r="H14" s="46">
         <v>0.499</v>
       </c>
-      <c r="I14" s="76"/>
+      <c r="I14" s="145"/>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -16408,21 +16397,21 @@
       <c r="D15" s="27">
         <v>0</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="85">
-        <v>0</v>
-      </c>
-      <c r="G15" s="85">
-        <v>0</v>
-      </c>
-      <c r="H15" s="85">
-        <v>0</v>
-      </c>
-      <c r="I15" s="76"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="79">
+        <v>0</v>
+      </c>
+      <c r="G15" s="79">
+        <v>0</v>
+      </c>
+      <c r="H15" s="79">
+        <v>0</v>
+      </c>
+      <c r="I15" s="145"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="144" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -16431,7 +16420,7 @@
       <c r="D16" s="15">
         <v>0</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="145"/>
       <c r="F16" s="46">
         <v>-0.70599999999999996</v>
       </c>
@@ -16441,17 +16430,17 @@
       <c r="H16" s="46">
         <v>2E-3</v>
       </c>
-      <c r="I16" s="76"/>
+      <c r="I16" s="145"/>
     </row>
     <row r="17" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="75"/>
+      <c r="B17" s="144"/>
       <c r="C17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="15">
         <v>0</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="145"/>
       <c r="F17" s="46">
         <v>-0.49199999999999999</v>
       </c>
@@ -16461,18 +16450,18 @@
       <c r="H17" s="46">
         <v>0.13300000000000001</v>
       </c>
-      <c r="I17" s="76"/>
+      <c r="I17" s="145"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="75"/>
+      <c r="B18" s="144"/>
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="15">
         <v>0</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="145"/>
       <c r="F18" s="46">
         <v>-0.628</v>
       </c>
@@ -16482,17 +16471,17 @@
       <c r="H18" s="46">
         <v>0.502</v>
       </c>
-      <c r="I18" s="76"/>
+      <c r="I18" s="145"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="75"/>
+      <c r="B19" s="144"/>
       <c r="C19" s="21" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="22">
         <v>0</v>
       </c>
-      <c r="E19" s="76"/>
+      <c r="E19" s="145"/>
       <c r="F19" s="46">
         <v>0.45600000000000002</v>
       </c>
@@ -16502,17 +16491,17 @@
       <c r="H19" s="46">
         <v>-0.629</v>
       </c>
-      <c r="I19" s="76"/>
+      <c r="I19" s="145"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="75"/>
+      <c r="B20" s="144"/>
       <c r="C20" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="22">
         <v>0</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="145"/>
       <c r="F20" s="46">
         <v>0.34799999999999998</v>
       </c>
@@ -16522,17 +16511,17 @@
       <c r="H20" s="46">
         <v>-0.74</v>
       </c>
-      <c r="I20" s="76"/>
+      <c r="I20" s="145"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="75"/>
+      <c r="B21" s="144"/>
       <c r="C21" s="39" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="22">
         <v>0</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="145"/>
       <c r="F21" s="46">
         <v>-0.627</v>
       </c>
@@ -16542,7 +16531,7 @@
       <c r="H21" s="46">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I21" s="76"/>
+      <c r="I21" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -16614,7 +16603,7 @@
       <c r="B6" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="103">
         <f>Sheet3_new!G6</f>
         <v>-0.46094526202756914</v>
       </c>
@@ -16627,13 +16616,13 @@
       <c r="G6" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="133">
+      <c r="H6" s="123">
         <v>-1.3173811656478494E-2</v>
       </c>
-      <c r="I6" s="133">
+      <c r="I6" s="123">
         <v>-0.17887373739259194</v>
       </c>
-      <c r="J6" s="133">
+      <c r="J6" s="123">
         <v>0.16121781289960807</v>
       </c>
     </row>
@@ -16837,20 +16826,20 @@
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="110">
+      <c r="C16" s="104">
         <f>Sheet3_new!G16</f>
         <v>0.47457641801215467</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="134">
+      <c r="H16" s="124">
         <v>1.3563389978232171E-2</v>
       </c>
-      <c r="I16" s="134">
+      <c r="I16" s="124">
         <v>0.18416342364561689</v>
       </c>
-      <c r="J16" s="134">
+      <c r="J16" s="124">
         <v>-0.16598537498596452</v>
       </c>
     </row>
@@ -16858,20 +16847,20 @@
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="111">
+      <c r="C17" s="105">
         <f>Sheet3_new!G17</f>
         <v>0.3683142284896011</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="135">
+      <c r="H17" s="125">
         <v>1.0526417508187742E-2</v>
       </c>
-      <c r="I17" s="135">
+      <c r="I17" s="125">
         <v>0.14292747536878603</v>
       </c>
-      <c r="J17" s="135">
+      <c r="J17" s="125">
         <v>-0.12881966530192593</v>
       </c>
     </row>
@@ -16879,20 +16868,20 @@
       <c r="B18" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="112">
+      <c r="C18" s="106">
         <f>Sheet3_new!G18</f>
         <v>0.48622150153162152</v>
       </c>
       <c r="G18" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="136">
+      <c r="H18" s="126">
         <v>1.3896206365875706E-2</v>
       </c>
-      <c r="I18" s="136">
+      <c r="I18" s="126">
         <v>0.18868239755200519</v>
       </c>
-      <c r="J18" s="136">
+      <c r="J18" s="126">
         <v>-0.17005829871617836</v>
       </c>
     </row>
@@ -16934,13 +16923,13 @@
         <f t="array" ref="C5:C18">error_new</f>
         <v>0.42642426569174846</v>
       </c>
-      <c r="E5" s="81">
-        <v>0</v>
-      </c>
-      <c r="F5" s="81">
-        <v>0</v>
-      </c>
-      <c r="G5" s="81">
+      <c r="E5" s="75">
+        <v>0</v>
+      </c>
+      <c r="F5" s="75">
+        <v>0</v>
+      </c>
+      <c r="G5" s="75">
         <v>0</v>
       </c>
       <c r="I5" s="36" t="s">
@@ -16954,18 +16943,18 @@
       <c r="B6" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="103">
         <v>-0.46094526202756914</v>
       </c>
-      <c r="E6" s="140">
+      <c r="E6" s="130">
         <f>Sheet2_new!B6</f>
         <v>0.74299999999999999</v>
       </c>
-      <c r="F6" s="140">
+      <c r="F6" s="130">
         <f>Sheet2_new!C6</f>
         <v>-0.39400000000000002</v>
       </c>
-      <c r="G6" s="140">
+      <c r="G6" s="130">
         <f>Sheet2_new!D6</f>
         <v>-0.82399999999999995</v>
       </c>
@@ -16983,13 +16972,13 @@
       <c r="C7" s="45">
         <v>0.46803773503295143</v>
       </c>
-      <c r="E7" s="81">
-        <v>0</v>
-      </c>
-      <c r="F7" s="81">
-        <v>0</v>
-      </c>
-      <c r="G7" s="81">
+      <c r="E7" s="75">
+        <v>0</v>
+      </c>
+      <c r="F7" s="75">
+        <v>0</v>
+      </c>
+      <c r="G7" s="75">
         <v>0</v>
       </c>
       <c r="I7" s="36" t="s">
@@ -17006,13 +16995,13 @@
       <c r="C8" s="45">
         <v>0.35570525000900333</v>
       </c>
-      <c r="E8" s="81">
-        <v>0</v>
-      </c>
-      <c r="F8" s="81">
-        <v>0</v>
-      </c>
-      <c r="G8" s="81">
+      <c r="E8" s="75">
+        <v>0</v>
+      </c>
+      <c r="F8" s="75">
+        <v>0</v>
+      </c>
+      <c r="G8" s="75">
         <v>0</v>
       </c>
       <c r="I8" s="36" t="s">
@@ -17029,26 +17018,26 @@
       <c r="C9" s="45">
         <v>0.48268217569896038</v>
       </c>
-      <c r="E9" s="81">
-        <v>0</v>
-      </c>
-      <c r="F9" s="81">
-        <v>0</v>
-      </c>
-      <c r="G9" s="81">
+      <c r="E9" s="75">
+        <v>0</v>
+      </c>
+      <c r="F9" s="75">
+        <v>0</v>
+      </c>
+      <c r="G9" s="75">
         <v>0</v>
       </c>
       <c r="I9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="111">
         <f t="array" ref="J9:L9">MMULT(TRANSPOSE(error_new), vec_out_new)</f>
         <v>-0.84312667485840065</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="111">
         <v>-0.14834054443585459</v>
       </c>
-      <c r="L9" s="117">
+      <c r="L9" s="111">
         <v>0.75564644684852766</v>
       </c>
     </row>
@@ -17060,22 +17049,22 @@
         <v>0.62945487515866361</v>
       </c>
       <c r="D10" s="68"/>
-      <c r="E10" s="81">
-        <v>0</v>
-      </c>
-      <c r="F10" s="81">
-        <v>0</v>
-      </c>
-      <c r="G10" s="81">
+      <c r="E10" s="75">
+        <v>0</v>
+      </c>
+      <c r="F10" s="75">
+        <v>0</v>
+      </c>
+      <c r="G10" s="75">
         <v>0</v>
       </c>
       <c r="H10" s="68"/>
       <c r="I10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="21" t="s">
@@ -17084,13 +17073,13 @@
       <c r="C11" s="45">
         <v>0.47955966626707563</v>
       </c>
-      <c r="E11" s="81">
-        <v>0</v>
-      </c>
-      <c r="F11" s="81">
-        <v>0</v>
-      </c>
-      <c r="G11" s="81">
+      <c r="E11" s="75">
+        <v>0</v>
+      </c>
+      <c r="F11" s="75">
+        <v>0</v>
+      </c>
+      <c r="G11" s="75">
         <v>0</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -17107,13 +17096,13 @@
       <c r="C12" s="45">
         <v>0.5</v>
       </c>
-      <c r="E12" s="81">
-        <v>0</v>
-      </c>
-      <c r="F12" s="81">
-        <v>0</v>
-      </c>
-      <c r="G12" s="81">
+      <c r="E12" s="75">
+        <v>0</v>
+      </c>
+      <c r="F12" s="75">
+        <v>0</v>
+      </c>
+      <c r="G12" s="75">
         <v>0</v>
       </c>
       <c r="I12" s="43">
@@ -17130,13 +17119,13 @@
       <c r="C13" s="45">
         <v>0.53690909392132258</v>
       </c>
-      <c r="E13" s="81">
-        <v>0</v>
-      </c>
-      <c r="F13" s="81">
-        <v>0</v>
-      </c>
-      <c r="G13" s="81">
+      <c r="E13" s="75">
+        <v>0</v>
+      </c>
+      <c r="F13" s="75">
+        <v>0</v>
+      </c>
+      <c r="G13" s="75">
         <v>0</v>
       </c>
       <c r="I13" s="21" t="s">
@@ -17153,13 +17142,13 @@
       <c r="C14" s="45">
         <v>0.51648502541186203</v>
       </c>
-      <c r="E14" s="81">
-        <v>0</v>
-      </c>
-      <c r="F14" s="81">
-        <v>0</v>
-      </c>
-      <c r="G14" s="81">
+      <c r="E14" s="75">
+        <v>0</v>
+      </c>
+      <c r="F14" s="75">
+        <v>0</v>
+      </c>
+      <c r="G14" s="75">
         <v>0</v>
       </c>
       <c r="I14" s="21" t="s">
@@ -17176,13 +17165,13 @@
       <c r="C15" s="45">
         <v>0.46645712144536033</v>
       </c>
-      <c r="E15" s="81">
-        <v>0</v>
-      </c>
-      <c r="F15" s="81">
-        <v>0</v>
-      </c>
-      <c r="G15" s="81">
+      <c r="E15" s="75">
+        <v>0</v>
+      </c>
+      <c r="F15" s="75">
+        <v>0</v>
+      </c>
+      <c r="G15" s="75">
         <v>0</v>
       </c>
       <c r="I15" s="21" t="s">
@@ -17196,18 +17185,18 @@
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="110">
+      <c r="C16" s="104">
         <v>0.47457641801215467</v>
       </c>
-      <c r="E16" s="137">
+      <c r="E16" s="127">
         <f>Sheet2_new!B16</f>
         <v>-2.8000000000000001E-2</v>
       </c>
-      <c r="F16" s="137">
+      <c r="F16" s="127">
         <f>Sheet2_new!C16</f>
         <v>-0.24399999999999999</v>
       </c>
-      <c r="G16" s="137">
+      <c r="G16" s="127">
         <f>Sheet2_new!D16</f>
         <v>1.7999999999999999E-2</v>
       </c>
@@ -17222,18 +17211,18 @@
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="111">
+      <c r="C17" s="105">
         <v>0.3683142284896011</v>
       </c>
-      <c r="E17" s="138">
+      <c r="E17" s="128">
         <f>Sheet2_new!B17</f>
         <v>-0.41099999999999998</v>
       </c>
-      <c r="F17" s="138">
+      <c r="F17" s="128">
         <f>Sheet2_new!C17</f>
         <v>-0.89300000000000002</v>
       </c>
-      <c r="G17" s="138">
+      <c r="G17" s="128">
         <f>Sheet2_new!D17</f>
         <v>0.51800000000000002</v>
       </c>
@@ -17248,18 +17237,18 @@
       <c r="B18" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="112">
+      <c r="C18" s="106">
         <v>0.48622150153162152</v>
       </c>
-      <c r="E18" s="139">
+      <c r="E18" s="129">
         <f>Sheet2_new!B18</f>
         <v>-0.69099999999999995</v>
       </c>
-      <c r="F18" s="139">
+      <c r="F18" s="129">
         <f>Sheet2_new!C18</f>
         <v>0.23599999999999999</v>
       </c>
-      <c r="G18" s="139">
+      <c r="G18" s="129">
         <f>Sheet2_new!D18</f>
         <v>0.36299999999999999</v>
       </c>
@@ -17271,14 +17260,14 @@
       <c r="L18" s="53"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="23"/>
@@ -17295,8 +17284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6EB33-7D04-43B0-BE3F-FDCA046B6F56}">
   <dimension ref="B4:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -17460,34 +17449,34 @@
       <c r="B9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="111">
         <v>2.8579991469118448E-2</v>
       </c>
-      <c r="D9" s="117">
+      <c r="D9" s="111">
         <v>0.38805852262322094</v>
       </c>
-      <c r="E9" s="117">
+      <c r="E9" s="111">
         <v>-0.34975478908375379</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="111">
         <f t="array" ref="I9:K9">MMULT(TRANSPOSE(error_new), vec_out_new)</f>
         <v>-0.84312667485840065</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="111">
         <v>-0.14834054443585459</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="111">
         <v>0.75564644684852766</v>
       </c>
-      <c r="M9" s="117">
+      <c r="M9" s="111">
         <f t="shared" si="0"/>
         <v>7.0736325212038487E-2</v>
       </c>
-      <c r="N9" s="117">
+      <c r="N9" s="111">
         <f t="shared" si="0"/>
         <v>0.39547554984501365</v>
       </c>
-      <c r="O9" s="117">
+      <c r="O9" s="111">
         <f t="shared" si="0"/>
         <v>-0.38753711142618019</v>
       </c>
@@ -17566,13 +17555,13 @@
       <c r="B12" s="43">
         <v>0</v>
       </c>
-      <c r="C12" s="85">
-        <v>0</v>
-      </c>
-      <c r="D12" s="85">
-        <v>0</v>
-      </c>
-      <c r="E12" s="85">
+      <c r="C12" s="79">
+        <v>0</v>
+      </c>
+      <c r="D12" s="79">
+        <v>0</v>
+      </c>
+      <c r="E12" s="79">
         <v>0</v>
       </c>
       <c r="I12" s="56">
@@ -17584,15 +17573,15 @@
       <c r="K12" s="56">
         <v>0</v>
       </c>
-      <c r="M12" s="85">
+      <c r="M12" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="85">
+      <c r="N12" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" s="85">
+      <c r="O12" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17867,27 +17856,27 @@
       <c r="E24" s="57">
         <v>-0.82399999999999995</v>
       </c>
-      <c r="I24" s="143">
+      <c r="I24" s="133">
         <f>Sheet4_new!H6</f>
         <v>-1.3173811656478494E-2</v>
       </c>
-      <c r="J24" s="143">
+      <c r="J24" s="133">
         <f>Sheet4_new!I6</f>
         <v>-0.17887373739259194</v>
       </c>
-      <c r="K24" s="143">
+      <c r="K24" s="133">
         <f>Sheet4_new!J6</f>
         <v>0.16121781289960807</v>
       </c>
-      <c r="M24" s="147">
+      <c r="M24" s="137">
         <f t="shared" ref="M24:M36" si="2">C24-$G$23*I24</f>
         <v>0.74365869058282397</v>
       </c>
-      <c r="N24" s="147">
+      <c r="N24" s="137">
         <f t="shared" si="1"/>
         <v>-0.38505631313037042</v>
       </c>
-      <c r="O24" s="147">
+      <c r="O24" s="137">
         <f t="shared" si="1"/>
         <v>-0.83206089064498034</v>
       </c>
@@ -18019,15 +18008,15 @@
       <c r="K28" s="60">
         <v>0</v>
       </c>
-      <c r="M28" s="82">
+      <c r="M28" s="76">
         <f t="shared" si="2"/>
         <v>0.11566199177815567</v>
       </c>
-      <c r="N28" s="82">
+      <c r="N28" s="76">
         <f t="shared" si="1"/>
         <v>0.73058640675695063</v>
       </c>
-      <c r="O28" s="82">
+      <c r="O28" s="76">
         <f t="shared" si="1"/>
         <v>-0.69495270035136969</v>
       </c>
@@ -18071,13 +18060,13 @@
       <c r="B30" s="43">
         <v>0</v>
       </c>
-      <c r="C30" s="86">
-        <v>0</v>
-      </c>
-      <c r="D30" s="86">
-        <v>0</v>
-      </c>
-      <c r="E30" s="86">
+      <c r="C30" s="80">
+        <v>0</v>
+      </c>
+      <c r="D30" s="80">
+        <v>0</v>
+      </c>
+      <c r="E30" s="80">
         <v>0</v>
       </c>
       <c r="I30" s="60">
@@ -18089,15 +18078,15 @@
       <c r="K30" s="60">
         <v>0</v>
       </c>
-      <c r="M30" s="86">
+      <c r="M30" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N30" s="86">
+      <c r="N30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O30" s="86">
+      <c r="O30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -18124,15 +18113,15 @@
       <c r="K31" s="60">
         <v>0</v>
       </c>
-      <c r="M31" s="82">
+      <c r="M31" s="76">
         <f t="shared" si="2"/>
         <v>-0.93950215704596762</v>
       </c>
-      <c r="N31" s="82">
+      <c r="N31" s="76">
         <f t="shared" si="1"/>
         <v>0.58982619147616244</v>
       </c>
-      <c r="O31" s="82">
+      <c r="O31" s="76">
         <f t="shared" si="1"/>
         <v>0.15476756757934779</v>
       </c>
@@ -18159,15 +18148,15 @@
       <c r="K32" s="60">
         <v>0</v>
       </c>
-      <c r="M32" s="82">
+      <c r="M32" s="76">
         <f t="shared" si="2"/>
         <v>-0.62151945603625103</v>
       </c>
-      <c r="N32" s="82">
+      <c r="N32" s="76">
         <f t="shared" si="1"/>
         <v>0.80021445770252408</v>
       </c>
-      <c r="O32" s="82">
+      <c r="O32" s="76">
         <f t="shared" si="1"/>
         <v>0.64846291313935622</v>
       </c>
@@ -18194,15 +18183,15 @@
       <c r="K33" s="60">
         <v>0</v>
       </c>
-      <c r="M33" s="82">
+      <c r="M33" s="76">
         <f t="shared" si="2"/>
         <v>-7.6579738045871051E-2</v>
       </c>
-      <c r="N33" s="82">
+      <c r="N33" s="76">
         <f t="shared" si="1"/>
         <v>-0.38443254608156086</v>
       </c>
-      <c r="O33" s="82">
+      <c r="O33" s="76">
         <f t="shared" si="1"/>
         <v>-4.8598720030062395E-2</v>
       </c>
@@ -18220,27 +18209,27 @@
       <c r="E34" s="57">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I34" s="144">
+      <c r="I34" s="134">
         <f>Sheet4_new!H16</f>
         <v>1.3563389978232171E-2</v>
       </c>
-      <c r="J34" s="144">
+      <c r="J34" s="134">
         <f>Sheet4_new!I16</f>
         <v>0.18416342364561689</v>
       </c>
-      <c r="K34" s="144">
+      <c r="K34" s="134">
         <f>Sheet4_new!J16</f>
         <v>-0.16598537498596452</v>
       </c>
-      <c r="M34" s="148">
+      <c r="M34" s="138">
         <f t="shared" si="2"/>
         <v>-2.867816949891161E-2</v>
       </c>
-      <c r="N34" s="148">
+      <c r="N34" s="138">
         <f t="shared" si="1"/>
         <v>-0.25320817118228084</v>
       </c>
-      <c r="O34" s="148">
+      <c r="O34" s="138">
         <f t="shared" si="1"/>
         <v>2.6299268749298225E-2</v>
       </c>
@@ -18258,27 +18247,27 @@
       <c r="E35" s="57">
         <v>0.51800000000000002</v>
       </c>
-      <c r="I35" s="145">
+      <c r="I35" s="135">
         <f>Sheet4_new!H17</f>
         <v>1.0526417508187742E-2</v>
       </c>
-      <c r="J35" s="145">
+      <c r="J35" s="135">
         <f>Sheet4_new!I17</f>
         <v>0.14292747536878603</v>
       </c>
-      <c r="K35" s="145">
+      <c r="K35" s="135">
         <f>Sheet4_new!J17</f>
         <v>-0.12881966530192593</v>
       </c>
-      <c r="M35" s="149">
+      <c r="M35" s="139">
         <f t="shared" si="2"/>
         <v>-0.41152632087540936</v>
       </c>
-      <c r="N35" s="149">
+      <c r="N35" s="139">
         <f t="shared" si="1"/>
         <v>-0.90014637376843931</v>
       </c>
-      <c r="O35" s="149">
+      <c r="O35" s="139">
         <f t="shared" si="1"/>
         <v>0.52444098326509636</v>
       </c>
@@ -18296,35 +18285,35 @@
       <c r="E36" s="57">
         <v>0.36299999999999999</v>
       </c>
-      <c r="I36" s="146">
+      <c r="I36" s="136">
         <f>Sheet4_new!H18</f>
         <v>1.3896206365875706E-2</v>
       </c>
-      <c r="J36" s="146">
+      <c r="J36" s="136">
         <f>Sheet4_new!I18</f>
         <v>0.18868239755200519</v>
       </c>
-      <c r="K36" s="146">
+      <c r="K36" s="136">
         <f>Sheet4_new!J18</f>
         <v>-0.17005829871617836</v>
       </c>
-      <c r="M36" s="150">
+      <c r="M36" s="140">
         <f t="shared" si="2"/>
         <v>-0.69169481031829372</v>
       </c>
-      <c r="N36" s="150">
+      <c r="N36" s="140">
         <f t="shared" si="1"/>
         <v>0.22656588012239973</v>
       </c>
-      <c r="O36" s="150">
+      <c r="O36" s="140">
         <f t="shared" si="1"/>
         <v>0.37150291493580889</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="77"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="I38" s="23"/>
@@ -18360,9 +18349,9 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
@@ -18385,12 +18374,12 @@
       <c r="D5" s="47">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="146"/>
       <c r="F5" s="29">
         <f>Sheet1!J8</f>
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="G5" s="77"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="12" t="s">
         <v>14</v>
       </c>
@@ -18414,12 +18403,12 @@
       <c r="D6" s="47">
         <v>-0.82399999999999995</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="146"/>
       <c r="F6" s="29">
         <f>Sheet1!J9</f>
         <v>0.40400000000000003</v>
       </c>
-      <c r="G6" s="77"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="26" t="s">
         <v>15</v>
       </c>
@@ -18444,12 +18433,12 @@
       <c r="D7" s="47">
         <v>-0.56399999999999995</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="146"/>
       <c r="F7" s="29">
         <f>Sheet1!J10</f>
         <v>-0.317</v>
       </c>
-      <c r="G7" s="77"/>
+      <c r="G7" s="146"/>
       <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
@@ -18474,8 +18463,8 @@
       <c r="D8" s="47">
         <v>0.89500000000000002</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="G8" s="77"/>
+      <c r="E8" s="146"/>
+      <c r="G8" s="146"/>
       <c r="H8" s="12" t="s">
         <v>16</v>
       </c>
@@ -18498,8 +18487,8 @@
       <c r="D9" s="47">
         <v>-0.501</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="G9" s="77"/>
+      <c r="E9" s="146"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="19" t="s">
         <v>17</v>
       </c>
@@ -18522,16 +18511,16 @@
       <c r="D10" s="47">
         <v>-0.68899999999999995</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="G10" s="77"/>
+      <c r="E10" s="146"/>
+      <c r="G10" s="146"/>
       <c r="H10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="90">
+      <c r="I10" s="84">
         <v>0.50841700000000001</v>
       </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="91">
+      <c r="K10" s="85">
         <f t="shared" si="0"/>
         <v>0.62443530906184719</v>
       </c>
@@ -18546,8 +18535,8 @@
       <c r="D11" s="47">
         <v>-0.34100000000000003</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="G11" s="77"/>
+      <c r="E11" s="146"/>
+      <c r="G11" s="146"/>
       <c r="H11" s="8" t="s">
         <v>5</v>
       </c>
@@ -18561,17 +18550,17 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="86">
-        <v>0</v>
-      </c>
-      <c r="C12" s="86">
-        <v>0</v>
-      </c>
-      <c r="D12" s="86">
-        <v>0</v>
-      </c>
-      <c r="E12" s="77"/>
-      <c r="G12" s="77"/>
+      <c r="B12" s="80">
+        <v>0</v>
+      </c>
+      <c r="C12" s="80">
+        <v>0</v>
+      </c>
+      <c r="D12" s="80">
+        <v>0</v>
+      </c>
+      <c r="E12" s="146"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="28">
         <v>0</v>
       </c>
@@ -18594,16 +18583,16 @@
       <c r="D13" s="47">
         <v>0.14599999999999999</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="G13" s="77"/>
+      <c r="E13" s="146"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="87">
+      <c r="I13" s="81">
         <v>0.21344200000000002</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" s="92">
+      <c r="K13" s="86">
         <f t="shared" si="0"/>
         <v>0.5531588378137412</v>
       </c>
@@ -18618,16 +18607,16 @@
       <c r="D14" s="47">
         <v>0.64</v>
       </c>
-      <c r="E14" s="77"/>
-      <c r="G14" s="77"/>
+      <c r="E14" s="146"/>
+      <c r="G14" s="146"/>
       <c r="H14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="88">
+      <c r="I14" s="82">
         <v>0.13596000000000003</v>
       </c>
       <c r="J14" s="6"/>
-      <c r="K14" s="93">
+      <c r="K14" s="87">
         <f t="shared" si="0"/>
         <v>0.53393773749881146</v>
       </c>
@@ -18642,16 +18631,16 @@
       <c r="D15" s="47">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="G15" s="77"/>
+      <c r="E15" s="146"/>
+      <c r="G15" s="146"/>
       <c r="H15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="89">
+      <c r="I15" s="83">
         <v>-0.13236200000000004</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="94">
+      <c r="K15" s="88">
         <f t="shared" si="0"/>
         <v>0.46695772680994357</v>
       </c>
@@ -18666,8 +18655,8 @@
       <c r="D16" s="47">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="E16" s="146"/>
+      <c r="G16" s="146"/>
       <c r="H16" s="21" t="s">
         <v>9</v>
       </c>
@@ -18690,8 +18679,8 @@
       <c r="D17" s="47">
         <v>0.51800000000000002</v>
       </c>
-      <c r="E17" s="77"/>
-      <c r="G17" s="77"/>
+      <c r="E17" s="146"/>
+      <c r="G17" s="146"/>
       <c r="H17" s="21" t="s">
         <v>10</v>
       </c>
@@ -18714,8 +18703,8 @@
       <c r="D18" s="47">
         <v>0.36299999999999999</v>
       </c>
-      <c r="E18" s="77"/>
-      <c r="G18" s="77"/>
+      <c r="E18" s="146"/>
+      <c r="G18" s="146"/>
       <c r="H18" s="23" t="s">
         <v>12</v>
       </c>
@@ -18851,15 +18840,15 @@
       <c r="B10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="91">
+      <c r="C10" s="85">
         <f>Sheet2!K10</f>
         <v>0.62443530906184719</v>
       </c>
       <c r="D10" s="50"/>
-      <c r="E10" s="95">
+      <c r="E10" s="89">
         <v>1</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="92">
         <f t="shared" si="0"/>
         <v>-0.37556469093815281</v>
       </c>
@@ -18902,15 +18891,15 @@
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="92">
+      <c r="C13" s="86">
         <f>Sheet2!K13</f>
         <v>0.5531588378137412</v>
       </c>
       <c r="D13" s="50"/>
-      <c r="E13" s="96">
-        <v>0</v>
-      </c>
-      <c r="G13" s="99">
+      <c r="E13" s="90">
+        <v>0</v>
+      </c>
+      <c r="G13" s="93">
         <f t="shared" si="0"/>
         <v>0.5531588378137412</v>
       </c>
@@ -18919,7 +18908,7 @@
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="93">
+      <c r="C14" s="87">
         <f>Sheet2!K14</f>
         <v>0.53393773749881146</v>
       </c>
@@ -18927,7 +18916,7 @@
       <c r="E14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="100">
+      <c r="G14" s="94">
         <f t="shared" si="0"/>
         <v>0.53393773749881146</v>
       </c>
@@ -18936,15 +18925,15 @@
       <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="94">
+      <c r="C15" s="88">
         <f>Sheet2!K15</f>
         <v>0.46695772680994357</v>
       </c>
       <c r="D15" s="50"/>
-      <c r="E15" s="97">
-        <v>0</v>
-      </c>
-      <c r="G15" s="101">
+      <c r="E15" s="91">
+        <v>0</v>
+      </c>
+      <c r="G15" s="95">
         <f t="shared" si="0"/>
         <v>0.46695772680994357</v>
       </c>
@@ -19152,20 +19141,20 @@
       <c r="B10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="92">
         <f>Sheet3!G10</f>
         <v>-0.37556469093815281</v>
       </c>
       <c r="G10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H10" s="99">
         <v>6.7601644368867498E-3</v>
       </c>
-      <c r="I10" s="105">
+      <c r="I10" s="99">
         <v>-0.15172813513901376</v>
       </c>
-      <c r="J10" s="105">
+      <c r="J10" s="99">
         <v>0.11905400702739444</v>
       </c>
     </row>
@@ -19215,20 +19204,20 @@
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="102">
+      <c r="C13" s="96">
         <f>Sheet3!G13</f>
         <v>0.5531588378137412</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="100">
         <v>-9.9568590806473414E-3</v>
       </c>
-      <c r="I13" s="106">
+      <c r="I13" s="100">
         <v>0.22347617047675145</v>
       </c>
-      <c r="J13" s="106">
+      <c r="J13" s="100">
         <v>-0.17535135158695597</v>
       </c>
     </row>
@@ -19236,20 +19225,20 @@
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="103">
+      <c r="C14" s="97">
         <f>Sheet3!G14</f>
         <v>0.53393773749881146</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="107">
+      <c r="H14" s="101">
         <v>-9.6108792749786051E-3</v>
       </c>
-      <c r="I14" s="107">
+      <c r="I14" s="101">
         <v>0.21571084594951984</v>
       </c>
-      <c r="J14" s="107">
+      <c r="J14" s="101">
         <v>-0.16925826278712325</v>
       </c>
     </row>
@@ -19257,20 +19246,20 @@
       <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="104">
+      <c r="C15" s="98">
         <f>Sheet3!G15</f>
         <v>0.46695772680994357</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="108">
+      <c r="H15" s="102">
         <v>-8.4052390825789837E-3</v>
       </c>
-      <c r="I15" s="108">
+      <c r="I15" s="102">
         <v>0.18865092163121722</v>
       </c>
-      <c r="J15" s="108">
+      <c r="J15" s="102">
         <v>-0.14802559939875212</v>
       </c>
     </row>
@@ -19478,14 +19467,14 @@
       <c r="I9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="111">
         <f t="array" ref="J9:L9">MMULT(TRANSPOSE(error), vec_out)</f>
         <v>-0.93159982938236885</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="111">
         <v>0.31882954753558124</v>
       </c>
-      <c r="L9" s="117">
+      <c r="L9" s="111">
         <v>0.65509578167507598</v>
       </c>
     </row>
@@ -19493,19 +19482,19 @@
       <c r="B10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="103">
         <f>Sheet3!G10</f>
         <v>-0.37556469093815281</v>
       </c>
-      <c r="E10" s="116">
+      <c r="E10" s="110">
         <f>Sheet2!B10</f>
         <v>0.11600000000000001</v>
       </c>
-      <c r="F10" s="116">
+      <c r="F10" s="110">
         <f>Sheet2!C10</f>
         <v>0.72299999999999998</v>
       </c>
-      <c r="G10" s="116">
+      <c r="G10" s="110">
         <f>Sheet2!D10</f>
         <v>-0.68899999999999995</v>
       </c>
@@ -19566,19 +19555,19 @@
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="110">
+      <c r="C13" s="104">
         <f>Sheet3!G13</f>
         <v>0.5531588378137412</v>
       </c>
-      <c r="E13" s="113">
+      <c r="E13" s="107">
         <f>Sheet2!B13</f>
         <v>-0.94</v>
       </c>
-      <c r="F13" s="113">
+      <c r="F13" s="107">
         <f>Sheet2!C13</f>
         <v>0.60099999999999998</v>
       </c>
-      <c r="G13" s="113">
+      <c r="G13" s="107">
         <f>Sheet2!D13</f>
         <v>0.14599999999999999</v>
       </c>
@@ -19593,19 +19582,19 @@
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="111">
+      <c r="C14" s="105">
         <f>Sheet3!G14</f>
         <v>0.53393773749881146</v>
       </c>
-      <c r="E14" s="114">
+      <c r="E14" s="108">
         <f>Sheet2!B14</f>
         <v>-0.622</v>
       </c>
-      <c r="F14" s="114">
+      <c r="F14" s="108">
         <f>Sheet2!C14</f>
         <v>0.81100000000000005</v>
       </c>
-      <c r="G14" s="114">
+      <c r="G14" s="108">
         <f>Sheet2!D14</f>
         <v>0.64</v>
       </c>
@@ -19620,19 +19609,19 @@
       <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="112">
+      <c r="C15" s="106">
         <f>Sheet3!G15</f>
         <v>0.46695772680994357</v>
       </c>
-      <c r="E15" s="115">
+      <c r="E15" s="109">
         <f>Sheet2!B15</f>
         <v>-7.6999999999999999E-2</v>
       </c>
-      <c r="F15" s="115">
+      <c r="F15" s="109">
         <f>Sheet2!C15</f>
         <v>-0.375</v>
       </c>
-      <c r="G15" s="115">
+      <c r="G15" s="109">
         <f>Sheet2!D15</f>
         <v>-5.6000000000000001E-2</v>
       </c>
@@ -19722,8 +19711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874C7BB3-05C2-4503-80C6-7C4B183D41FA}">
   <dimension ref="B4:O36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -19886,34 +19875,34 @@
       <c r="B9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="151">
+      <c r="C9" s="141">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="D9" s="151">
+      <c r="D9" s="141">
         <v>0.40400000000000003</v>
       </c>
-      <c r="E9" s="151">
+      <c r="E9" s="141">
         <v>-0.317</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="111">
         <f t="array" ref="I9:K9">MMULT(TRANSPOSE(error), vec_out)</f>
         <v>-0.93159982938236885</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="111">
         <v>0.31882954753558124</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="111">
         <v>0.65509578167507598</v>
       </c>
-      <c r="M9" s="117">
+      <c r="M9" s="111">
         <f t="shared" si="0"/>
         <v>2.8579991469118448E-2</v>
       </c>
-      <c r="N9" s="117">
+      <c r="N9" s="111">
         <f t="shared" si="1"/>
         <v>0.38805852262322094</v>
       </c>
-      <c r="O9" s="117">
+      <c r="O9" s="111">
         <f t="shared" si="2"/>
         <v>-0.34975478908375379</v>
       </c>
@@ -19992,13 +19981,13 @@
       <c r="B12" s="43">
         <v>0</v>
       </c>
-      <c r="C12" s="85">
-        <v>0</v>
-      </c>
-      <c r="D12" s="85">
-        <v>0</v>
-      </c>
-      <c r="E12" s="85">
+      <c r="C12" s="79">
+        <v>0</v>
+      </c>
+      <c r="D12" s="79">
+        <v>0</v>
+      </c>
+      <c r="E12" s="79">
         <v>0</v>
       </c>
       <c r="I12" s="56">
@@ -20010,15 +19999,15 @@
       <c r="K12" s="56">
         <v>0</v>
       </c>
-      <c r="M12" s="85">
+      <c r="M12" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="85">
+      <c r="N12" s="79">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="85">
+      <c r="O12" s="79">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20258,13 +20247,13 @@
       <c r="G23" s="59">
         <v>0.05</v>
       </c>
-      <c r="I23" s="84">
-        <v>0</v>
-      </c>
-      <c r="J23" s="84">
-        <v>0</v>
-      </c>
-      <c r="K23" s="84">
+      <c r="I23" s="60">
+        <v>0</v>
+      </c>
+      <c r="J23" s="60">
+        <v>0</v>
+      </c>
+      <c r="K23" s="60">
         <v>0</v>
       </c>
       <c r="M23" s="57">
@@ -20293,13 +20282,13 @@
       <c r="E24" s="48">
         <v>-0.82399999999999995</v>
       </c>
-      <c r="I24" s="84">
-        <v>0</v>
-      </c>
-      <c r="J24" s="84">
-        <v>0</v>
-      </c>
-      <c r="K24" s="84">
+      <c r="I24" s="60">
+        <v>0</v>
+      </c>
+      <c r="J24" s="60">
+        <v>0</v>
+      </c>
+      <c r="K24" s="60">
         <v>0</v>
       </c>
       <c r="M24" s="57">
@@ -20328,13 +20317,13 @@
       <c r="E25" s="48">
         <v>-0.56399999999999995</v>
       </c>
-      <c r="I25" s="84">
-        <v>0</v>
-      </c>
-      <c r="J25" s="84">
-        <v>0</v>
-      </c>
-      <c r="K25" s="84">
+      <c r="I25" s="60">
+        <v>0</v>
+      </c>
+      <c r="J25" s="60">
+        <v>0</v>
+      </c>
+      <c r="K25" s="60">
         <v>0</v>
       </c>
       <c r="M25" s="57">
@@ -20363,13 +20352,13 @@
       <c r="E26" s="48">
         <v>0.89500000000000002</v>
       </c>
-      <c r="I26" s="84">
-        <v>0</v>
-      </c>
-      <c r="J26" s="84">
-        <v>0</v>
-      </c>
-      <c r="K26" s="84">
+      <c r="I26" s="60">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60">
+        <v>0</v>
+      </c>
+      <c r="K26" s="60">
         <v>0</v>
       </c>
       <c r="M26" s="57">
@@ -20398,13 +20387,13 @@
       <c r="E27" s="48">
         <v>-0.501</v>
       </c>
-      <c r="I27" s="84">
-        <v>0</v>
-      </c>
-      <c r="J27" s="84">
-        <v>0</v>
-      </c>
-      <c r="K27" s="84">
+      <c r="I27" s="60">
+        <v>0</v>
+      </c>
+      <c r="J27" s="60">
+        <v>0</v>
+      </c>
+      <c r="K27" s="60">
         <v>0</v>
       </c>
       <c r="M27" s="57">
@@ -20433,27 +20422,27 @@
       <c r="E28" s="48">
         <v>-0.68899999999999995</v>
       </c>
-      <c r="I28" s="119">
+      <c r="I28" s="133">
         <f>Sheet4!H10</f>
         <v>6.7601644368867498E-3</v>
       </c>
-      <c r="J28" s="119">
+      <c r="J28" s="133">
         <f>Sheet4!I10</f>
         <v>-0.15172813513901376</v>
       </c>
-      <c r="K28" s="119">
+      <c r="K28" s="133">
         <f>Sheet4!J10</f>
         <v>0.11905400702739444</v>
       </c>
-      <c r="M28" s="142">
+      <c r="M28" s="132">
         <f t="shared" si="4"/>
         <v>0.11566199177815567</v>
       </c>
-      <c r="N28" s="142">
+      <c r="N28" s="132">
         <f t="shared" si="5"/>
         <v>0.73058640675695063</v>
       </c>
-      <c r="O28" s="142">
+      <c r="O28" s="132">
         <f t="shared" si="6"/>
         <v>-0.69495270035136969</v>
       </c>
@@ -20471,24 +20460,24 @@
       <c r="E29" s="48">
         <v>-0.34100000000000003</v>
       </c>
-      <c r="I29" s="84">
-        <v>0</v>
-      </c>
-      <c r="J29" s="84">
-        <v>0</v>
-      </c>
-      <c r="K29" s="84">
-        <v>0</v>
-      </c>
-      <c r="M29" s="141">
+      <c r="I29" s="60">
+        <v>0</v>
+      </c>
+      <c r="J29" s="60">
+        <v>0</v>
+      </c>
+      <c r="K29" s="60">
+        <v>0</v>
+      </c>
+      <c r="M29" s="131">
         <f t="shared" si="4"/>
         <v>-0.16500000000000001</v>
       </c>
-      <c r="N29" s="141">
+      <c r="N29" s="131">
         <f t="shared" si="5"/>
         <v>-0.50600000000000001</v>
       </c>
-      <c r="O29" s="141">
+      <c r="O29" s="131">
         <f t="shared" si="6"/>
         <v>-0.34100000000000003</v>
       </c>
@@ -20497,33 +20486,33 @@
       <c r="B30" s="43">
         <v>0</v>
       </c>
-      <c r="C30" s="118">
-        <v>0</v>
-      </c>
-      <c r="D30" s="118">
-        <v>0</v>
-      </c>
-      <c r="E30" s="118">
-        <v>0</v>
-      </c>
-      <c r="I30" s="84">
-        <v>0</v>
-      </c>
-      <c r="J30" s="84">
-        <v>0</v>
-      </c>
-      <c r="K30" s="84">
-        <v>0</v>
-      </c>
-      <c r="M30" s="81">
+      <c r="C30" s="112">
+        <v>0</v>
+      </c>
+      <c r="D30" s="112">
+        <v>0</v>
+      </c>
+      <c r="E30" s="112">
+        <v>0</v>
+      </c>
+      <c r="I30" s="60">
+        <v>0</v>
+      </c>
+      <c r="J30" s="60">
+        <v>0</v>
+      </c>
+      <c r="K30" s="60">
+        <v>0</v>
+      </c>
+      <c r="M30" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N30" s="81">
+      <c r="N30" s="75">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O30" s="81">
+      <c r="O30" s="75">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -20541,15 +20530,15 @@
       <c r="E31" s="48">
         <v>0.14599999999999999</v>
       </c>
-      <c r="I31" s="120">
+      <c r="I31" s="134">
         <f>Sheet4!H13</f>
         <v>-9.9568590806473414E-3</v>
       </c>
-      <c r="J31" s="120">
+      <c r="J31" s="134">
         <f>Sheet4!I13</f>
         <v>0.22347617047675145</v>
       </c>
-      <c r="K31" s="120">
+      <c r="K31" s="134">
         <f>Sheet4!J13</f>
         <v>-0.17535135158695597</v>
       </c>
@@ -20579,15 +20568,15 @@
       <c r="E32" s="48">
         <v>0.64</v>
       </c>
-      <c r="I32" s="121">
+      <c r="I32" s="135">
         <f>Sheet4!H14</f>
         <v>-9.6108792749786051E-3</v>
       </c>
-      <c r="J32" s="121">
+      <c r="J32" s="135">
         <f>Sheet4!I14</f>
         <v>0.21571084594951984</v>
       </c>
-      <c r="K32" s="121">
+      <c r="K32" s="135">
         <f>Sheet4!J14</f>
         <v>-0.16925826278712325</v>
       </c>
@@ -20617,15 +20606,15 @@
       <c r="E33" s="48">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="I33" s="122">
+      <c r="I33" s="136">
         <f>Sheet4!H15</f>
         <v>-8.4052390825789837E-3</v>
       </c>
-      <c r="J33" s="122">
+      <c r="J33" s="136">
         <f>Sheet4!I15</f>
         <v>0.18865092163121722</v>
       </c>
-      <c r="K33" s="122">
+      <c r="K33" s="136">
         <f>Sheet4!J15</f>
         <v>-0.14802559939875212</v>
       </c>
@@ -20655,13 +20644,13 @@
       <c r="E34" s="48">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I34" s="84">
-        <v>0</v>
-      </c>
-      <c r="J34" s="84">
-        <v>0</v>
-      </c>
-      <c r="K34" s="84">
+      <c r="I34" s="78">
+        <v>0</v>
+      </c>
+      <c r="J34" s="78">
+        <v>0</v>
+      </c>
+      <c r="K34" s="78">
         <v>0</v>
       </c>
       <c r="M34" s="57">
@@ -20690,13 +20679,13 @@
       <c r="E35" s="48">
         <v>0.51800000000000002</v>
       </c>
-      <c r="I35" s="84">
-        <v>0</v>
-      </c>
-      <c r="J35" s="84">
-        <v>0</v>
-      </c>
-      <c r="K35" s="84">
+      <c r="I35" s="78">
+        <v>0</v>
+      </c>
+      <c r="J35" s="78">
+        <v>0</v>
+      </c>
+      <c r="K35" s="78">
         <v>0</v>
       </c>
       <c r="M35" s="57">
@@ -20725,13 +20714,13 @@
       <c r="E36" s="48">
         <v>0.36299999999999999</v>
       </c>
-      <c r="I36" s="84">
-        <v>0</v>
-      </c>
-      <c r="J36" s="84">
-        <v>0</v>
-      </c>
-      <c r="K36" s="84">
+      <c r="I36" s="78">
+        <v>0</v>
+      </c>
+      <c r="J36" s="78">
+        <v>0</v>
+      </c>
+      <c r="K36" s="78">
         <v>0</v>
       </c>
       <c r="M36" s="57">
@@ -20771,43 +20760,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
     </row>
     <row r="4" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
     </row>
     <row r="5" spans="2:10" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
     </row>
     <row r="6" spans="2:10" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1"/>
@@ -20848,7 +20837,7 @@
       <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E8" s="76"/>
+      <c r="E8" s="145"/>
       <c r="F8" s="46">
         <f>Sheet6!M5</f>
         <v>-1.4E-2</v>
@@ -20861,7 +20850,7 @@
         <f>Sheet6!O5</f>
         <v>0.109</v>
       </c>
-      <c r="I8" s="76"/>
+      <c r="I8" s="145"/>
       <c r="J8" s="7">
         <f t="array" ref="J8:J10">TRANSPOSE(MMULT(TRANSPOSE(input), w_input))</f>
         <v>2.8579991469118448E-2</v>
@@ -20877,7 +20866,7 @@
       <c r="D9" s="14">
         <v>0</v>
       </c>
-      <c r="E9" s="76"/>
+      <c r="E9" s="145"/>
       <c r="F9" s="46">
         <f>Sheet6!M6</f>
         <v>-0.66500000000000004</v>
@@ -20890,7 +20879,7 @@
         <f>Sheet6!O6</f>
         <v>0.309</v>
       </c>
-      <c r="I9" s="76"/>
+      <c r="I9" s="145"/>
       <c r="J9" s="7">
         <v>0.38805852262322094</v>
       </c>
@@ -20905,7 +20894,7 @@
       <c r="D10" s="11">
         <v>0</v>
       </c>
-      <c r="E10" s="76"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="46">
         <f>Sheet6!M7</f>
         <v>0.70199999999999996</v>
@@ -20918,7 +20907,7 @@
         <f>Sheet6!O7</f>
         <v>-0.98099999999999998</v>
       </c>
-      <c r="I10" s="76"/>
+      <c r="I10" s="145"/>
       <c r="J10" s="7">
         <v>-0.34975478908375379</v>
       </c>
@@ -20933,7 +20922,7 @@
       <c r="D11" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="76"/>
+      <c r="E11" s="145"/>
       <c r="F11" s="46">
         <f>Sheet6!M8</f>
         <v>0.214</v>
@@ -20946,7 +20935,7 @@
         <f>Sheet6!O8</f>
         <v>-0.56100000000000005</v>
       </c>
-      <c r="I11" s="76"/>
+      <c r="I11" s="145"/>
       <c r="J11" s="24"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -20959,20 +20948,20 @@
       <c r="D12" s="20">
         <v>1</v>
       </c>
-      <c r="E12" s="76"/>
-      <c r="F12" s="151">
+      <c r="E12" s="145"/>
+      <c r="F12" s="141">
         <f>Sheet6!M9</f>
         <v>2.8579991469118448E-2</v>
       </c>
-      <c r="G12" s="151">
+      <c r="G12" s="141">
         <f>Sheet6!N9</f>
         <v>0.38805852262322094</v>
       </c>
-      <c r="H12" s="151">
+      <c r="H12" s="141">
         <f>Sheet6!O9</f>
         <v>-0.34975478908375379</v>
       </c>
-      <c r="I12" s="76"/>
+      <c r="I12" s="145"/>
       <c r="J12" s="24"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -20985,7 +20974,7 @@
       <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E13" s="76"/>
+      <c r="E13" s="145"/>
       <c r="F13" s="46">
         <f>Sheet6!M10</f>
         <v>0.20399999999999999</v>
@@ -20998,7 +20987,7 @@
         <f>Sheet6!O10</f>
         <v>-0.73299999999999998</v>
       </c>
-      <c r="I13" s="76"/>
+      <c r="I13" s="145"/>
       <c r="J13" s="24"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -21011,7 +21000,7 @@
       <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="76"/>
+      <c r="E14" s="145"/>
       <c r="F14" s="46">
         <f>Sheet6!M11</f>
         <v>-0.65200000000000002</v>
@@ -21024,7 +21013,7 @@
         <f>Sheet6!O11</f>
         <v>0.499</v>
       </c>
-      <c r="I14" s="76"/>
+      <c r="I14" s="145"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -21033,24 +21022,24 @@
       <c r="D15" s="27">
         <v>0</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="85">
+      <c r="E15" s="145"/>
+      <c r="F15" s="79">
         <f>Sheet6!M12</f>
         <v>0</v>
       </c>
-      <c r="G15" s="85">
+      <c r="G15" s="79">
         <f>Sheet6!N12</f>
         <v>0</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="79">
         <f>Sheet6!O12</f>
         <v>0</v>
       </c>
-      <c r="I15" s="76"/>
+      <c r="I15" s="145"/>
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="144" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -21059,7 +21048,7 @@
       <c r="D16" s="9">
         <v>0</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="145"/>
       <c r="F16" s="46">
         <f>Sheet6!M13</f>
         <v>-0.70599999999999996</v>
@@ -21072,17 +21061,17 @@
         <f>Sheet6!O13</f>
         <v>2E-3</v>
       </c>
-      <c r="I16" s="76"/>
+      <c r="I16" s="145"/>
     </row>
     <row r="17" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="75"/>
+      <c r="B17" s="144"/>
       <c r="C17" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="145"/>
       <c r="F17" s="46">
         <f>Sheet6!M14</f>
         <v>-0.49199999999999999</v>
@@ -21095,18 +21084,18 @@
         <f>Sheet6!O14</f>
         <v>0.13300000000000001</v>
       </c>
-      <c r="I17" s="76"/>
+      <c r="I17" s="145"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="75"/>
+      <c r="B18" s="144"/>
       <c r="C18" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="145"/>
       <c r="F18" s="46">
         <f>Sheet6!M15</f>
         <v>-0.628</v>
@@ -21119,17 +21108,17 @@
         <f>Sheet6!O15</f>
         <v>0.502</v>
       </c>
-      <c r="I18" s="76"/>
+      <c r="I18" s="145"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="75"/>
+      <c r="B19" s="144"/>
       <c r="C19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="63">
         <v>0</v>
       </c>
-      <c r="E19" s="76"/>
+      <c r="E19" s="145"/>
       <c r="F19" s="46">
         <f>Sheet6!M16</f>
         <v>0.45600000000000002</v>
@@ -21142,17 +21131,17 @@
         <f>Sheet6!O16</f>
         <v>-0.629</v>
       </c>
-      <c r="I19" s="76"/>
+      <c r="I19" s="145"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="75"/>
+      <c r="B20" s="144"/>
       <c r="C20" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="63">
         <v>0</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="145"/>
       <c r="F20" s="46">
         <f>Sheet6!M17</f>
         <v>0.34799999999999998</v>
@@ -21165,17 +21154,17 @@
         <f>Sheet6!O17</f>
         <v>-0.74</v>
       </c>
-      <c r="I20" s="76"/>
+      <c r="I20" s="145"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="75"/>
+      <c r="B21" s="144"/>
       <c r="C21" s="64" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="63">
         <v>0</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="145"/>
       <c r="F21" s="46">
         <f>Sheet6!M18</f>
         <v>-0.627</v>
@@ -21188,7 +21177,7 @@
         <f>Sheet6!O18</f>
         <v>0.46600000000000003</v>
       </c>
-      <c r="I21" s="76"/>
+      <c r="I21" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -21222,9 +21211,9 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
@@ -21250,12 +21239,12 @@
         <f>Sheet6!O23</f>
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="146"/>
       <c r="F5" s="55">
         <f>Sheet1_new!J8</f>
         <v>2.8579991469118448E-2</v>
       </c>
-      <c r="G5" s="77"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="12" t="s">
         <v>14</v>
       </c>
@@ -21282,22 +21271,22 @@
         <f>Sheet6!O24</f>
         <v>-0.82399999999999995</v>
       </c>
-      <c r="E6" s="77"/>
+      <c r="E6" s="146"/>
       <c r="F6" s="55">
         <f>Sheet1_new!J9</f>
         <v>0.38805852262322094</v>
       </c>
-      <c r="G6" s="77"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="123">
+      <c r="I6" s="113">
         <v>0.15653782195301907</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="91">
+      <c r="K6" s="85">
         <f t="shared" ref="K6:K18" si="0">1/(1+EXP(-I6))</f>
         <v>0.53905473797243086</v>
       </c>
@@ -21315,12 +21304,12 @@
         <f>Sheet6!O25</f>
         <v>-0.56399999999999995</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="146"/>
       <c r="F7" s="55">
         <f>Sheet1_new!J10</f>
         <v>-0.34975478908375379</v>
       </c>
-      <c r="G7" s="77"/>
+      <c r="G7" s="146"/>
       <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
@@ -21348,8 +21337,8 @@
         <f>Sheet6!O26</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="G8" s="77"/>
+      <c r="E8" s="146"/>
+      <c r="G8" s="146"/>
       <c r="H8" s="12" t="s">
         <v>16</v>
       </c>
@@ -21375,8 +21364,8 @@
         <f>Sheet6!O27</f>
         <v>-0.501</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="G9" s="77"/>
+      <c r="E9" s="146"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="19" t="s">
         <v>17</v>
       </c>
@@ -21402,8 +21391,8 @@
         <f>Sheet6!O28</f>
         <v>-0.69495270035136969</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="G10" s="77"/>
+      <c r="E10" s="146"/>
+      <c r="G10" s="146"/>
       <c r="H10" s="8" t="s">
         <v>18</v>
       </c>
@@ -21429,8 +21418,8 @@
         <f>Sheet6!O29</f>
         <v>-0.34100000000000003</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="G11" s="77"/>
+      <c r="E11" s="146"/>
+      <c r="G11" s="146"/>
       <c r="H11" s="8" t="s">
         <v>5</v>
       </c>
@@ -21444,20 +21433,20 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="86">
+      <c r="B12" s="80">
         <f>Sheet6!M30</f>
         <v>0</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="80">
         <f>Sheet6!N30</f>
         <v>0</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="80">
         <f>Sheet6!O30</f>
         <v>0</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="G12" s="77"/>
+      <c r="E12" s="146"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="28">
         <v>0</v>
       </c>
@@ -21483,8 +21472,8 @@
         <f>Sheet6!O31</f>
         <v>0.15476756757934779</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="G13" s="77"/>
+      <c r="E13" s="146"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="21" t="s">
         <v>6</v>
       </c>
@@ -21510,8 +21499,8 @@
         <f>Sheet6!O32</f>
         <v>0.64846291313935622</v>
       </c>
-      <c r="E14" s="77"/>
-      <c r="G14" s="77"/>
+      <c r="E14" s="146"/>
+      <c r="G14" s="146"/>
       <c r="H14" s="21" t="s">
         <v>11</v>
       </c>
@@ -21537,8 +21526,8 @@
         <f>Sheet6!O33</f>
         <v>-4.8598720030062395E-2</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="G15" s="77"/>
+      <c r="E15" s="146"/>
+      <c r="G15" s="146"/>
       <c r="H15" s="21" t="s">
         <v>7</v>
       </c>
@@ -21564,16 +21553,16 @@
         <f>Sheet6!O34</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="E16" s="146"/>
+      <c r="G16" s="146"/>
       <c r="H16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="124">
+      <c r="I16" s="114">
         <v>-0.10178210548470878</v>
       </c>
       <c r="J16" s="24"/>
-      <c r="K16" s="127">
+      <c r="K16" s="117">
         <f t="shared" si="0"/>
         <v>0.47457641801215467</v>
       </c>
@@ -21591,16 +21580,16 @@
         <f>Sheet6!O35</f>
         <v>0.51800000000000002</v>
       </c>
-      <c r="E17" s="77"/>
-      <c r="G17" s="77"/>
+      <c r="E17" s="146"/>
+      <c r="G17" s="146"/>
       <c r="H17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="125">
+      <c r="I17" s="115">
         <v>-0.53945561794172847</v>
       </c>
       <c r="J17" s="24"/>
-      <c r="K17" s="128">
+      <c r="K17" s="118">
         <f t="shared" si="0"/>
         <v>0.3683142284896011</v>
       </c>
@@ -21618,16 +21607,16 @@
         <f>Sheet6!O36</f>
         <v>0.36299999999999999</v>
       </c>
-      <c r="E18" s="77"/>
-      <c r="G18" s="77"/>
+      <c r="E18" s="146"/>
+      <c r="G18" s="146"/>
       <c r="H18" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="126">
+      <c r="I18" s="116">
         <v>-5.5127951203483322E-2</v>
       </c>
       <c r="J18" s="24"/>
-      <c r="K18" s="129">
+      <c r="K18" s="119">
         <f t="shared" si="0"/>
         <v>0.48622150153162152</v>
       </c>
@@ -21787,16 +21776,16 @@
       <c r="B6" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="91">
+      <c r="C6" s="85">
         <f>Sheet2_new!K6</f>
         <v>0.53905473797243086</v>
       </c>
       <c r="D6" s="70"/>
-      <c r="E6" s="95">
+      <c r="E6" s="89">
         <v>1</v>
       </c>
       <c r="F6" s="35"/>
-      <c r="G6" s="98">
+      <c r="G6" s="92">
         <f t="shared" si="0"/>
         <v>-0.46094526202756914</v>
       </c>
@@ -21959,15 +21948,15 @@
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="92">
+      <c r="C16" s="86">
         <f>Sheet2_new!K16</f>
         <v>0.47457641801215467</v>
       </c>
       <c r="D16" s="50"/>
-      <c r="E16" s="130">
-        <v>0</v>
-      </c>
-      <c r="G16" s="99">
+      <c r="E16" s="120">
+        <v>0</v>
+      </c>
+      <c r="G16" s="93">
         <f t="shared" si="0"/>
         <v>0.47457641801215467</v>
       </c>
@@ -21976,15 +21965,15 @@
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="93">
+      <c r="C17" s="87">
         <f>Sheet2_new!K17</f>
         <v>0.3683142284896011</v>
       </c>
       <c r="D17" s="50"/>
-      <c r="E17" s="131">
-        <v>0</v>
-      </c>
-      <c r="G17" s="100">
+      <c r="E17" s="121">
+        <v>0</v>
+      </c>
+      <c r="G17" s="94">
         <f t="shared" si="0"/>
         <v>0.3683142284896011</v>
       </c>
@@ -21993,15 +21982,15 @@
       <c r="B18" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="94">
+      <c r="C18" s="88">
         <f>Sheet2_new!K18</f>
         <v>0.48622150153162152</v>
       </c>
       <c r="D18" s="50"/>
-      <c r="E18" s="132">
-        <v>0</v>
-      </c>
-      <c r="G18" s="101">
+      <c r="E18" s="122">
+        <v>0</v>
+      </c>
+      <c r="G18" s="95">
         <f t="shared" si="0"/>
         <v>0.48622150153162152</v>
       </c>

</xml_diff>